<commit_message>
Added SP800_85B tests that were not included in the various tabs, removed unneeded files.  Updates to the spreadsheet.
</commit_message>
<xml_diff>
--- a/docs/85b_test_definitions.xlsx
+++ b/docs/85b_test_definitions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\armen\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GSA\GSA_GIT\piv-conformance\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFC59F4E-7167-4A01-9D20-F00A08C5E8F4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10AADEC3-0056-4A73-AC6F-C4E54E5A80A3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="700">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="693">
   <si>
     <t>Test Case</t>
   </si>
@@ -1869,9 +1869,6 @@
     <t>CMS.10</t>
   </si>
   <si>
-    <t>Confirm that digestAlgorithm in signer info matches attribute from signedAttributes bag</t>
-  </si>
-  <si>
     <t>CMS.11</t>
   </si>
   <si>
@@ -2106,31 +2103,13 @@
     <t>Test is there but I'm not 100% sure if that is enough, might require additional checks</t>
   </si>
   <si>
-    <t>Test is pretty much there except I need to figure out how to squeeze curve name out of java or bouncy castle EC key</t>
-  </si>
-  <si>
-    <t>Yes (but same issue as with second SP800-78 test)</t>
-  </si>
-  <si>
-    <t>Test is there but I have a question if my assumption was correct</t>
-  </si>
-  <si>
-    <t>Test is there but I'm not sure how exactly to test this condition</t>
-  </si>
-  <si>
-    <t>Yes not sure about what is the oid for piv interim extension</t>
-  </si>
-  <si>
-    <t>Yes  but not sure about what is the oid for piv interim extension</t>
-  </si>
-  <si>
     <t>Test placeholder written but there is an outstanding question regarding this test</t>
   </si>
   <si>
-    <t>Test Atoms Exist</t>
-  </si>
-  <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>All Test Atoms Exist</t>
   </si>
 </sst>
 </file>
@@ -4408,7 +4387,7 @@
   <dimension ref="A1:E58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52:E58"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4435,7 +4414,7 @@
         <v>312</v>
       </c>
       <c r="E1" t="s">
-        <v>698</v>
+        <v>692</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
@@ -4452,7 +4431,7 @@
         <v>315</v>
       </c>
       <c r="E2" t="s">
-        <v>699</v>
+        <v>691</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
@@ -4469,7 +4448,7 @@
         <v>317</v>
       </c>
       <c r="E3" t="s">
-        <v>699</v>
+        <v>691</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
@@ -4486,7 +4465,7 @@
         <v>319</v>
       </c>
       <c r="E4" t="s">
-        <v>699</v>
+        <v>691</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -4503,7 +4482,7 @@
         <v>321</v>
       </c>
       <c r="E5" t="s">
-        <v>699</v>
+        <v>691</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
@@ -4520,7 +4499,7 @@
         <v>323</v>
       </c>
       <c r="E6" t="s">
-        <v>699</v>
+        <v>691</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -4537,7 +4516,7 @@
         <v>325</v>
       </c>
       <c r="E7" t="s">
-        <v>699</v>
+        <v>691</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
@@ -4554,7 +4533,7 @@
         <v>319</v>
       </c>
       <c r="E8" t="s">
-        <v>699</v>
+        <v>691</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
@@ -4571,7 +4550,7 @@
         <v>319</v>
       </c>
       <c r="E9" t="s">
-        <v>699</v>
+        <v>691</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
@@ -4588,7 +4567,7 @@
         <v>319</v>
       </c>
       <c r="E10" t="s">
-        <v>699</v>
+        <v>691</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -4605,7 +4584,7 @@
         <v>331</v>
       </c>
       <c r="E11" t="s">
-        <v>699</v>
+        <v>691</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -4622,7 +4601,7 @@
         <v>334</v>
       </c>
       <c r="E12" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -4639,7 +4618,7 @@
         <v>76.5</v>
       </c>
       <c r="E13" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -4656,7 +4635,7 @@
         <v>339</v>
       </c>
       <c r="E14" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
@@ -4673,7 +4652,7 @@
         <v>342</v>
       </c>
       <c r="E15" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
@@ -4687,7 +4666,7 @@
         <v>344</v>
       </c>
       <c r="E16" t="s">
-        <v>699</v>
+        <v>688</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
@@ -4701,7 +4680,7 @@
         <v>346</v>
       </c>
       <c r="E17" t="s">
-        <v>699</v>
+        <v>688</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -4718,7 +4697,7 @@
         <v>349</v>
       </c>
       <c r="E18" t="s">
-        <v>699</v>
+        <v>688</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -4732,7 +4711,7 @@
         <v>351</v>
       </c>
       <c r="E19" t="s">
-        <v>699</v>
+        <v>688</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
@@ -4746,7 +4725,7 @@
         <v>353</v>
       </c>
       <c r="E20" t="s">
-        <v>699</v>
+        <v>688</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -4760,7 +4739,7 @@
         <v>355</v>
       </c>
       <c r="E21" t="s">
-        <v>699</v>
+        <v>688</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
@@ -4774,7 +4753,7 @@
         <v>357</v>
       </c>
       <c r="E22" t="s">
-        <v>699</v>
+        <v>688</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
@@ -4788,7 +4767,7 @@
         <v>359</v>
       </c>
       <c r="E23" t="s">
-        <v>699</v>
+        <v>688</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -4802,7 +4781,7 @@
         <v>361</v>
       </c>
       <c r="E24" t="s">
-        <v>699</v>
+        <v>688</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
@@ -4819,7 +4798,7 @@
         <v>364</v>
       </c>
       <c r="E25" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
@@ -4836,7 +4815,7 @@
         <v>367</v>
       </c>
       <c r="E26" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -4853,7 +4832,7 @@
         <v>339</v>
       </c>
       <c r="E27" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
@@ -4870,7 +4849,7 @@
         <v>342</v>
       </c>
       <c r="E28" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
@@ -4884,7 +4863,7 @@
         <v>371</v>
       </c>
       <c r="E29" t="s">
-        <v>699</v>
+        <v>688</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
@@ -4898,7 +4877,7 @@
         <v>346</v>
       </c>
       <c r="E30" t="s">
-        <v>699</v>
+        <v>688</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -4915,7 +4894,7 @@
         <v>374</v>
       </c>
       <c r="E31" t="s">
-        <v>699</v>
+        <v>688</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -4929,7 +4908,7 @@
         <v>376</v>
       </c>
       <c r="E32" t="s">
-        <v>699</v>
+        <v>688</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
@@ -4943,7 +4922,7 @@
         <v>378</v>
       </c>
       <c r="E33" t="s">
-        <v>699</v>
+        <v>688</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -4957,7 +4936,7 @@
         <v>355</v>
       </c>
       <c r="E34" t="s">
-        <v>699</v>
+        <v>688</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
@@ -4971,7 +4950,7 @@
         <v>357</v>
       </c>
       <c r="E35" t="s">
-        <v>699</v>
+        <v>688</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
@@ -4985,7 +4964,7 @@
         <v>359</v>
       </c>
       <c r="E36" t="s">
-        <v>699</v>
+        <v>688</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -4999,7 +4978,7 @@
         <v>361</v>
       </c>
       <c r="E37" t="s">
-        <v>699</v>
+        <v>688</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
@@ -5016,7 +4995,7 @@
         <v>385</v>
       </c>
       <c r="E38" t="s">
-        <v>699</v>
+        <v>688</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
@@ -5033,7 +5012,7 @@
         <v>388</v>
       </c>
       <c r="E39" t="s">
-        <v>699</v>
+        <v>688</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
@@ -5050,7 +5029,7 @@
         <v>391</v>
       </c>
       <c r="E40" t="s">
-        <v>699</v>
+        <v>691</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
@@ -5067,7 +5046,7 @@
         <v>394</v>
       </c>
       <c r="E41" t="s">
-        <v>699</v>
+        <v>688</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -5084,7 +5063,7 @@
         <v>397</v>
       </c>
       <c r="E42" t="s">
-        <v>699</v>
+        <v>688</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
@@ -5101,7 +5080,7 @@
         <v>400</v>
       </c>
       <c r="E43" t="s">
-        <v>699</v>
+        <v>688</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -5118,7 +5097,7 @@
         <v>403</v>
       </c>
       <c r="E44" t="s">
-        <v>699</v>
+        <v>688</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
@@ -5135,7 +5114,7 @@
         <v>406</v>
       </c>
       <c r="E45" t="s">
-        <v>699</v>
+        <v>688</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -5152,7 +5131,7 @@
         <v>403</v>
       </c>
       <c r="E46" t="s">
-        <v>699</v>
+        <v>688</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
@@ -5169,7 +5148,7 @@
         <v>406</v>
       </c>
       <c r="E47" t="s">
-        <v>699</v>
+        <v>688</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -5186,7 +5165,7 @@
         <v>403</v>
       </c>
       <c r="E48" t="s">
-        <v>699</v>
+        <v>688</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
@@ -5203,7 +5182,7 @@
         <v>415</v>
       </c>
       <c r="E49" t="s">
-        <v>699</v>
+        <v>691</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -5220,7 +5199,7 @@
         <v>418</v>
       </c>
       <c r="E50" t="s">
-        <v>699</v>
+        <v>688</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -5237,7 +5216,7 @@
         <v>421</v>
       </c>
       <c r="E51" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
@@ -5254,7 +5233,7 @@
         <v>424</v>
       </c>
       <c r="E52" t="s">
-        <v>699</v>
+        <v>688</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -5271,7 +5250,7 @@
         <v>421</v>
       </c>
       <c r="E53" t="s">
-        <v>699</v>
+        <v>688</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -5288,7 +5267,7 @@
         <v>429</v>
       </c>
       <c r="E54" t="s">
-        <v>699</v>
+        <v>688</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -5305,7 +5284,7 @@
         <v>421</v>
       </c>
       <c r="E55" t="s">
-        <v>699</v>
+        <v>688</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -5322,7 +5301,7 @@
         <v>434</v>
       </c>
       <c r="E56" t="s">
-        <v>699</v>
+        <v>688</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -5339,7 +5318,7 @@
         <v>421</v>
       </c>
       <c r="E57" t="s">
-        <v>699</v>
+        <v>688</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
@@ -5356,12 +5335,12 @@
         <v>439</v>
       </c>
       <c r="E58" t="s">
-        <v>699</v>
+        <v>688</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5370,7 +5349,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5388,7 +5367,7 @@
         <v>311</v>
       </c>
       <c r="C1" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -5399,7 +5378,7 @@
         <v>442</v>
       </c>
       <c r="C2" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -5410,7 +5389,7 @@
         <v>444</v>
       </c>
       <c r="C3" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -5421,7 +5400,7 @@
         <v>446</v>
       </c>
       <c r="C4" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -5432,7 +5411,7 @@
         <v>448</v>
       </c>
       <c r="C5" t="s">
-        <v>697</v>
+        <v>690</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -5443,7 +5422,7 @@
         <v>450</v>
       </c>
       <c r="C6" t="s">
-        <v>697</v>
+        <v>688</v>
       </c>
     </row>
   </sheetData>
@@ -5457,7 +5436,7 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5478,7 +5457,7 @@
         <v>451</v>
       </c>
       <c r="D1" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5492,7 +5471,7 @@
         <v>454</v>
       </c>
       <c r="D2" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5506,7 +5485,7 @@
         <v>454</v>
       </c>
       <c r="D3" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -5520,7 +5499,7 @@
         <v>454</v>
       </c>
       <c r="D4" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -5535,7 +5514,7 @@
         <v>454</v>
       </c>
       <c r="D5" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -5550,7 +5529,7 @@
         <v>454</v>
       </c>
       <c r="D6" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -5564,7 +5543,7 @@
         <v>463</v>
       </c>
       <c r="D7" t="s">
-        <v>697</v>
+        <v>690</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -5578,7 +5557,7 @@
         <v>454</v>
       </c>
       <c r="D8" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -5592,7 +5571,7 @@
         <v>454</v>
       </c>
       <c r="D9" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -5606,7 +5585,7 @@
         <v>454</v>
       </c>
       <c r="D10" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -5620,7 +5599,7 @@
         <v>454</v>
       </c>
       <c r="D11" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -5634,7 +5613,7 @@
         <v>454</v>
       </c>
       <c r="D12" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -5648,7 +5627,7 @@
         <v>454</v>
       </c>
       <c r="D13" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -5662,7 +5641,7 @@
         <v>454</v>
       </c>
       <c r="D14" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -5676,7 +5655,7 @@
         <v>454</v>
       </c>
       <c r="D15" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -5690,7 +5669,7 @@
         <v>454</v>
       </c>
       <c r="D16" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -5704,7 +5683,7 @@
         <v>454</v>
       </c>
       <c r="D17" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -5718,7 +5697,7 @@
         <v>454</v>
       </c>
       <c r="D18" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -5732,7 +5711,7 @@
         <v>454</v>
       </c>
       <c r="D19" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -5746,7 +5725,7 @@
         <v>454</v>
       </c>
       <c r="D20" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -5760,7 +5739,7 @@
         <v>454</v>
       </c>
       <c r="D21" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -5774,7 +5753,7 @@
         <v>454</v>
       </c>
       <c r="D22" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -5788,7 +5767,7 @@
         <v>454</v>
       </c>
       <c r="D23" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -5802,7 +5781,7 @@
         <v>454</v>
       </c>
       <c r="D24" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -5816,7 +5795,7 @@
         <v>454</v>
       </c>
       <c r="D25" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -5830,7 +5809,7 @@
         <v>454</v>
       </c>
       <c r="D26" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -5844,7 +5823,7 @@
         <v>454</v>
       </c>
       <c r="D27" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -5858,7 +5837,7 @@
         <v>454</v>
       </c>
       <c r="D28" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -5872,7 +5851,7 @@
         <v>454</v>
       </c>
       <c r="D29" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -5886,7 +5865,7 @@
         <v>454</v>
       </c>
       <c r="D30" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -5900,7 +5879,7 @@
         <v>454</v>
       </c>
       <c r="D31" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -5914,7 +5893,7 @@
         <v>454</v>
       </c>
       <c r="D32" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -5928,7 +5907,7 @@
         <v>454</v>
       </c>
       <c r="D33" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -5942,7 +5921,7 @@
         <v>454</v>
       </c>
       <c r="D34" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -5953,7 +5932,7 @@
         <v>519</v>
       </c>
       <c r="D35" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -5964,7 +5943,7 @@
         <v>521</v>
       </c>
       <c r="D36" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -5975,7 +5954,7 @@
         <v>523</v>
       </c>
       <c r="D37" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
   </sheetData>
@@ -5989,7 +5968,7 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C27" sqref="C27:C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6007,7 +5986,7 @@
         <v>311</v>
       </c>
       <c r="C1" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -6018,7 +5997,7 @@
         <v>524</v>
       </c>
       <c r="C2" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -6029,7 +6008,7 @@
         <v>526</v>
       </c>
       <c r="C3" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -6040,7 +6019,7 @@
         <v>528</v>
       </c>
       <c r="C4" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6051,7 +6030,7 @@
         <v>530</v>
       </c>
       <c r="C5" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -6062,7 +6041,7 @@
         <v>531</v>
       </c>
       <c r="C6" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -6073,7 +6052,7 @@
         <v>532</v>
       </c>
       <c r="C7" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -6084,7 +6063,7 @@
         <v>533</v>
       </c>
       <c r="C8" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6095,7 +6074,7 @@
         <v>535</v>
       </c>
       <c r="C9" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -6103,10 +6082,10 @@
         <v>536</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="C10" t="s">
-        <v>693</v>
+        <v>688</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -6117,7 +6096,7 @@
         <v>538</v>
       </c>
       <c r="C11" t="s">
-        <v>693</v>
+        <v>688</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -6128,7 +6107,7 @@
         <v>540</v>
       </c>
       <c r="C12" t="s">
-        <v>694</v>
+        <v>688</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6139,7 +6118,7 @@
         <v>542</v>
       </c>
       <c r="C13" t="s">
-        <v>693</v>
+        <v>688</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -6150,7 +6129,7 @@
         <v>544</v>
       </c>
       <c r="C14" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -6161,7 +6140,7 @@
         <v>546</v>
       </c>
       <c r="C15" t="s">
-        <v>693</v>
+        <v>688</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6172,7 +6151,7 @@
         <v>548</v>
       </c>
       <c r="C16" t="s">
-        <v>697</v>
+        <v>688</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -6183,7 +6162,7 @@
         <v>550</v>
       </c>
       <c r="C17" t="s">
-        <v>697</v>
+        <v>688</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -6194,7 +6173,7 @@
         <v>552</v>
       </c>
       <c r="C18" t="s">
-        <v>697</v>
+        <v>688</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -6205,7 +6184,7 @@
         <v>554</v>
       </c>
       <c r="C19" t="s">
-        <v>697</v>
+        <v>688</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -6216,7 +6195,7 @@
         <v>556</v>
       </c>
       <c r="C20" t="s">
-        <v>697</v>
+        <v>688</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -6227,7 +6206,7 @@
         <v>558</v>
       </c>
       <c r="C21" t="s">
-        <v>697</v>
+        <v>688</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -6238,7 +6217,7 @@
         <v>560</v>
       </c>
       <c r="C22" t="s">
-        <v>697</v>
+        <v>688</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -6249,7 +6228,7 @@
         <v>562</v>
       </c>
       <c r="C23" t="s">
-        <v>697</v>
+        <v>688</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -6260,7 +6239,7 @@
         <v>564</v>
       </c>
       <c r="C24" t="s">
-        <v>697</v>
+        <v>688</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -6271,7 +6250,7 @@
         <v>566</v>
       </c>
       <c r="C25" t="s">
-        <v>697</v>
+        <v>688</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -6282,7 +6261,7 @@
         <v>568</v>
       </c>
       <c r="C26" t="s">
-        <v>697</v>
+        <v>690</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -6293,7 +6272,7 @@
         <v>570</v>
       </c>
       <c r="C27" t="s">
-        <v>697</v>
+        <v>688</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -6304,7 +6283,7 @@
         <v>572</v>
       </c>
       <c r="C28" t="s">
-        <v>697</v>
+        <v>688</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -6315,7 +6294,7 @@
         <v>574</v>
       </c>
       <c r="C29" t="s">
-        <v>697</v>
+        <v>688</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -6326,7 +6305,7 @@
         <v>576</v>
       </c>
       <c r="C30" t="s">
-        <v>697</v>
+        <v>688</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -6337,7 +6316,7 @@
         <v>578</v>
       </c>
       <c r="C31" t="s">
-        <v>697</v>
+        <v>688</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -6348,7 +6327,7 @@
         <v>580</v>
       </c>
       <c r="C32" t="s">
-        <v>697</v>
+        <v>688</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -6359,7 +6338,7 @@
         <v>582</v>
       </c>
       <c r="C33" t="s">
-        <v>697</v>
+        <v>688</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -6370,7 +6349,7 @@
         <v>584</v>
       </c>
       <c r="C34" t="s">
-        <v>697</v>
+        <v>688</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -6381,7 +6360,7 @@
         <v>586</v>
       </c>
       <c r="C35" t="s">
-        <v>697</v>
+        <v>688</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -6392,7 +6371,7 @@
         <v>588</v>
       </c>
       <c r="C36" t="s">
-        <v>697</v>
+        <v>688</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -6403,7 +6382,7 @@
         <v>590</v>
       </c>
       <c r="C37" t="s">
-        <v>697</v>
+        <v>688</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -6414,7 +6393,7 @@
         <v>592</v>
       </c>
       <c r="C38" t="s">
-        <v>697</v>
+        <v>688</v>
       </c>
     </row>
   </sheetData>
@@ -6428,7 +6407,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6447,7 +6426,7 @@
         <v>311</v>
       </c>
       <c r="C1" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6458,7 +6437,7 @@
         <v>594</v>
       </c>
       <c r="C2" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6469,7 +6448,7 @@
         <v>596</v>
       </c>
       <c r="C3" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -6480,7 +6459,7 @@
         <v>598</v>
       </c>
       <c r="C4" t="s">
-        <v>697</v>
+        <v>688</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -6491,7 +6470,7 @@
         <v>600</v>
       </c>
       <c r="C5" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -6502,7 +6481,7 @@
         <v>602</v>
       </c>
       <c r="C6" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -6513,7 +6492,7 @@
         <v>604</v>
       </c>
       <c r="C7" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -6524,7 +6503,7 @@
         <v>606</v>
       </c>
       <c r="C8" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -6535,7 +6514,7 @@
         <v>608</v>
       </c>
       <c r="C9" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -6546,7 +6525,7 @@
         <v>610</v>
       </c>
       <c r="C10" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -6554,117 +6533,153 @@
         <v>611</v>
       </c>
       <c r="B11" t="s">
-        <v>612</v>
+        <v>664</v>
       </c>
       <c r="C11" t="s">
-        <v>696</v>
+        <v>688</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>612</v>
+      </c>
+      <c r="B12" t="s">
         <v>613</v>
       </c>
-      <c r="B12" t="s">
-        <v>614</v>
+      <c r="C12" t="s">
+        <v>688</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>614</v>
+      </c>
+      <c r="B13" t="s">
         <v>615</v>
       </c>
-      <c r="B13" t="s">
-        <v>616</v>
+      <c r="C13" t="s">
+        <v>688</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
+        <v>616</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>617</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="C14" t="s">
+        <v>688</v>
+      </c>
+      <c r="D14" t="s">
         <v>618</v>
-      </c>
-      <c r="D14" t="s">
-        <v>619</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>619</v>
+      </c>
+      <c r="B15" t="s">
         <v>620</v>
       </c>
-      <c r="B15" t="s">
-        <v>621</v>
+      <c r="C15" t="s">
+        <v>688</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>621</v>
+      </c>
+      <c r="B16" t="s">
         <v>622</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>623</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
         <v>624</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>625</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="B18" t="s">
         <v>626</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>627</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B19" t="s">
         <v>628</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>629</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="B20" t="s">
         <v>630</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>631</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="B21" t="s">
         <v>632</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>633</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="B22" t="s">
         <v>634</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>635</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="B23" t="s">
         <v>636</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>637</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="B24" t="s">
         <v>638</v>
-      </c>
-      <c r="B24" t="s">
-        <v>639</v>
       </c>
     </row>
   </sheetData>
@@ -6678,7 +6693,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6696,40 +6711,40 @@
         <v>311</v>
       </c>
       <c r="C1" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>640</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>641</v>
-      </c>
       <c r="C2" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>642</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>643</v>
-      </c>
       <c r="C3" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>643</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>644</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>645</v>
-      </c>
       <c r="C4" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
   </sheetData>
@@ -6742,8 +6757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6761,7 +6776,7 @@
         <v>311</v>
       </c>
       <c r="C1" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6769,225 +6784,225 @@
         <v>421</v>
       </c>
       <c r="B2" t="s">
+        <v>645</v>
+      </c>
+      <c r="C2" t="s">
+        <v>688</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>646</v>
-      </c>
-      <c r="C2" t="s">
-        <v>692</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>647</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>647</v>
+      </c>
+      <c r="B3" t="s">
         <v>648</v>
       </c>
-      <c r="B3" t="s">
-        <v>649</v>
-      </c>
       <c r="C3" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>649</v>
+      </c>
+      <c r="B4" t="s">
         <v>650</v>
       </c>
-      <c r="B4" t="s">
-        <v>651</v>
-      </c>
       <c r="C4" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>651</v>
+      </c>
+      <c r="B5" t="s">
         <v>652</v>
       </c>
-      <c r="B5" t="s">
-        <v>653</v>
-      </c>
       <c r="C5" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>653</v>
+      </c>
+      <c r="B6" t="s">
         <v>654</v>
       </c>
-      <c r="B6" t="s">
-        <v>655</v>
-      </c>
       <c r="C6" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>655</v>
+      </c>
+      <c r="B7" t="s">
         <v>656</v>
       </c>
-      <c r="B7" t="s">
-        <v>657</v>
-      </c>
       <c r="C7" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>657</v>
+      </c>
+      <c r="B8" t="s">
         <v>658</v>
       </c>
-      <c r="B8" t="s">
-        <v>659</v>
-      </c>
       <c r="C8" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>659</v>
+      </c>
+      <c r="B9" t="s">
         <v>660</v>
       </c>
-      <c r="B9" t="s">
-        <v>661</v>
-      </c>
       <c r="C9" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>661</v>
+      </c>
+      <c r="B10" t="s">
         <v>662</v>
       </c>
-      <c r="B10" t="s">
-        <v>663</v>
-      </c>
       <c r="C10" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>663</v>
+      </c>
+      <c r="B11" t="s">
         <v>664</v>
       </c>
-      <c r="B11" t="s">
-        <v>665</v>
-      </c>
       <c r="C11" t="s">
-        <v>695</v>
+        <v>688</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>665</v>
+      </c>
+      <c r="B12" t="s">
         <v>666</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
+        <v>688</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>667</v>
-      </c>
-      <c r="C12" t="s">
-        <v>689</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>668</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>668</v>
+      </c>
+      <c r="B13" t="s">
         <v>669</v>
       </c>
-      <c r="B13" t="s">
-        <v>670</v>
-      </c>
       <c r="C13" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>670</v>
+      </c>
+      <c r="B14" t="s">
         <v>671</v>
       </c>
-      <c r="B14" t="s">
-        <v>672</v>
-      </c>
       <c r="C14" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>672</v>
+      </c>
+      <c r="B15" t="s">
         <v>673</v>
       </c>
-      <c r="B15" t="s">
-        <v>674</v>
-      </c>
       <c r="C15" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>674</v>
+      </c>
+      <c r="B16" t="s">
         <v>675</v>
       </c>
-      <c r="B16" t="s">
-        <v>676</v>
-      </c>
       <c r="C16" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>676</v>
+      </c>
+      <c r="B17" t="s">
         <v>677</v>
       </c>
-      <c r="B17" t="s">
-        <v>678</v>
-      </c>
       <c r="C17" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>678</v>
+      </c>
+      <c r="B18" t="s">
         <v>679</v>
       </c>
-      <c r="B18" t="s">
-        <v>680</v>
-      </c>
       <c r="C18" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>680</v>
+      </c>
+      <c r="B19" t="s">
         <v>681</v>
       </c>
-      <c r="B19" t="s">
-        <v>682</v>
-      </c>
       <c r="C19" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>682</v>
+      </c>
+      <c r="B20" t="s">
         <v>683</v>
       </c>
-      <c r="B20" t="s">
-        <v>684</v>
-      </c>
       <c r="C20" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>684</v>
+      </c>
+      <c r="B21" t="s">
         <v>685</v>
       </c>
-      <c r="B21" t="s">
-        <v>686</v>
-      </c>
       <c r="C21" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
   </sheetData>

</xml_diff>